<commit_message>
Actualizacion del plan de pruebas
</commit_message>
<xml_diff>
--- a/Proyectos/Activos/Viaticos_q/3. Ejecución/3.3 Pruebas Internas/Viaticos_q_plan_de_pruebas.xlsx
+++ b/Proyectos/Activos/Viaticos_q/3. Ejecución/3.3 Pruebas Internas/Viaticos_q_plan_de_pruebas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Cliente</t>
   </si>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>Validar la visualizacion del contenido web en diversos dispositivos.</t>
+  </si>
+  <si>
+    <t>El usuario sera capaz de editar el estado de los gastos y viaticos del proyecto</t>
+  </si>
+  <si>
+    <t>CU06</t>
+  </si>
+  <si>
+    <t>Validar que el usuario puede generar cambios sobre el estado de viaticos y gastos</t>
   </si>
 </sst>
 </file>
@@ -336,7 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -392,6 +401,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -745,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="A9:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,15 +944,25 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
+    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="23" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>

</xml_diff>